<commit_message>
added coded for extract PDF
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -612,16 +612,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -670,7 +670,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="28.8">
+    <row r="4" spans="1:26" ht="30">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1689,12 +1689,12 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" style="6" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1731,7 +1731,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.4">
+    <row r="3" spans="1:26">
       <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
@@ -2856,16 +2856,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>